<commit_message>
created two scripts to search the local maxes of the batch size and error rate more exhaustively. check the excel file.
</commit_message>
<xml_diff>
--- a/torch_simulation/results/learning_rate_batch_size.xlsx
+++ b/torch_simulation/results/learning_rate_batch_size.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>Batch Size</t>
   </si>
@@ -55,12 +55,39 @@
   <si>
     <t>bad</t>
   </si>
+  <si>
+    <t>Average Accuracy</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>LOCAL MAX B:</t>
+  </si>
+  <si>
+    <t>LOCAL MAX A:</t>
+  </si>
+  <si>
+    <t>Local Max A Search Results</t>
+  </si>
+  <si>
+    <t>Local Max B Search Results</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Accuracy </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,8 +95,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,8 +131,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,17 +152,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,9 +761,839 @@
         <v>0.18865100000000001</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4">
+        <v>0.89549999999999996</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4">
+        <v>2.9149999999999999E-2</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4">
+        <v>8</v>
+      </c>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2">
+        <v>7</v>
+      </c>
+      <c r="E34" s="2">
+        <v>8</v>
+      </c>
+      <c r="F34" s="2">
+        <v>9</v>
+      </c>
+      <c r="G34" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C35">
+        <v>0.6925</v>
+      </c>
+      <c r="D35">
+        <v>0.86050000000000004</v>
+      </c>
+      <c r="E35">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="F35">
+        <v>0.86050000000000004</v>
+      </c>
+      <c r="G35">
+        <v>0.77200000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="3">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="C36">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="D36">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="E36">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="F36">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="G36">
+        <v>0.89300000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C37">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="D37">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="E37">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="F37">
+        <v>0.77249999999999996</v>
+      </c>
+      <c r="G37">
+        <v>0.73450000000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="3">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="C38">
+        <v>0.80349999999999999</v>
+      </c>
+      <c r="D38">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="E38">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="F38">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="G38">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="3">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="C39">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="D39">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E39">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="F39">
+        <v>0.754</v>
+      </c>
+      <c r="G39">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2">
+        <v>6</v>
+      </c>
+      <c r="D43" s="2">
+        <v>7</v>
+      </c>
+      <c r="E43" s="2">
+        <v>8</v>
+      </c>
+      <c r="F43" s="2">
+        <v>9</v>
+      </c>
+      <c r="G43" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C44">
+        <v>0.214</v>
+      </c>
+      <c r="D44">
+        <v>0.13805100000000001</v>
+      </c>
+      <c r="E44">
+        <v>0.12723599999999999</v>
+      </c>
+      <c r="F44">
+        <v>0.11390699999999999</v>
+      </c>
+      <c r="G44">
+        <v>0.15118400000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="3">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="C45">
+        <v>0.13312099999999999</v>
+      </c>
+      <c r="D45">
+        <v>0.12847</v>
+      </c>
+      <c r="E45">
+        <v>0.195658</v>
+      </c>
+      <c r="F45">
+        <v>0.20807600000000001</v>
+      </c>
+      <c r="G45">
+        <v>1.9606999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C46">
+        <v>0.16817599999999999</v>
+      </c>
+      <c r="D46">
+        <v>0.110222</v>
+      </c>
+      <c r="E46">
+        <v>0.19591900000000001</v>
+      </c>
+      <c r="F46">
+        <v>0.19421099999999999</v>
+      </c>
+      <c r="G46">
+        <v>0.21190200000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="3">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="C47">
+        <v>0.160001</v>
+      </c>
+      <c r="D47">
+        <v>0.147701</v>
+      </c>
+      <c r="E47">
+        <v>0.18152499999999999</v>
+      </c>
+      <c r="F47">
+        <v>0.143007</v>
+      </c>
+      <c r="G47">
+        <v>0.193692</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="3">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="C48">
+        <v>2.6693000000000001E-2</v>
+      </c>
+      <c r="D48">
+        <v>0.21396999999999999</v>
+      </c>
+      <c r="E48">
+        <v>0.16655400000000001</v>
+      </c>
+      <c r="F48">
+        <v>0.18387500000000001</v>
+      </c>
+      <c r="G48">
+        <v>0.20327899999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B51" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B52" s="4"/>
+      <c r="C52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4">
+        <v>0.89300000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4">
+        <v>1.9606999999999999E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54" s="4"/>
+      <c r="C54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4">
+        <v>2.2460000000000001E-2</v>
+      </c>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4">
+        <v>32</v>
+      </c>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="4"/>
+      <c r="D63" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2">
+        <v>30</v>
+      </c>
+      <c r="D69" s="2">
+        <v>31</v>
+      </c>
+      <c r="E69" s="2">
+        <v>32</v>
+      </c>
+      <c r="F69" s="2">
+        <v>33</v>
+      </c>
+      <c r="G69" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C70">
+        <v>0.77849999999999997</v>
+      </c>
+      <c r="D70">
+        <v>0.78549999999999998</v>
+      </c>
+      <c r="E70">
+        <v>0.78049999999999997</v>
+      </c>
+      <c r="F70">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="G70">
+        <v>0.70099999999999996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C71">
+        <v>0.78149999999999997</v>
+      </c>
+      <c r="D71">
+        <v>0.80449999999999999</v>
+      </c>
+      <c r="E71">
+        <v>0.78349999999999997</v>
+      </c>
+      <c r="F71">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="G71">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C72">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="D72">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="E72">
+        <v>0.82150000000000001</v>
+      </c>
+      <c r="F72">
+        <v>0.76649999999999996</v>
+      </c>
+      <c r="G72">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C73">
+        <v>0.71850000000000003</v>
+      </c>
+      <c r="D73">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="E73">
+        <v>0.73850000000000005</v>
+      </c>
+      <c r="F73">
+        <v>0.71450000000000002</v>
+      </c>
+      <c r="G73">
+        <v>0.77649999999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C74">
+        <v>0.74750000000000005</v>
+      </c>
+      <c r="D74">
+        <v>0.85650000000000004</v>
+      </c>
+      <c r="E74">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="F74">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="G74">
+        <v>0.78100000000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2">
+        <v>30</v>
+      </c>
+      <c r="D78" s="2">
+        <v>31</v>
+      </c>
+      <c r="E78" s="2">
+        <v>32</v>
+      </c>
+      <c r="F78" s="2">
+        <v>33</v>
+      </c>
+      <c r="G78" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C79">
+        <v>0.20269100000000001</v>
+      </c>
+      <c r="D79">
+        <v>0.173341</v>
+      </c>
+      <c r="E79">
+        <v>0.18656900000000001</v>
+      </c>
+      <c r="F79">
+        <v>0.16703000000000001</v>
+      </c>
+      <c r="G79">
+        <v>0.18285999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C80">
+        <v>0.187113</v>
+      </c>
+      <c r="D80">
+        <v>0.16908999999999999</v>
+      </c>
+      <c r="E80">
+        <v>0.19409399999999999</v>
+      </c>
+      <c r="F80">
+        <v>0.176789</v>
+      </c>
+      <c r="G80">
+        <v>0.15785399999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C81">
+        <v>0.19564999999999999</v>
+      </c>
+      <c r="D81">
+        <v>0.205343</v>
+      </c>
+      <c r="E81">
+        <v>0.171821</v>
+      </c>
+      <c r="F81">
+        <v>0.173846</v>
+      </c>
+      <c r="G81">
+        <v>0.19856099999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C82">
+        <v>0.19007399999999999</v>
+      </c>
+      <c r="D82">
+        <v>0.171124</v>
+      </c>
+      <c r="E82">
+        <v>0.216115</v>
+      </c>
+      <c r="F82">
+        <v>0.206592</v>
+      </c>
+      <c r="G82">
+        <v>0.177201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C83">
+        <v>0.17963299999999999</v>
+      </c>
+      <c r="D83">
+        <v>0.15726899999999999</v>
+      </c>
+      <c r="E83">
+        <v>0.181839</v>
+      </c>
+      <c r="F83">
+        <v>0.184944</v>
+      </c>
+      <c r="G83">
+        <v>0.19759399999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B86" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B87" s="4"/>
+      <c r="C87" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4">
+        <v>0.85650000000000004</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B88" s="4"/>
+      <c r="C88" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4">
+        <v>0.15726899999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B89" s="4"/>
+      <c r="C89" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B90" s="4"/>
+      <c r="C90" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C3:F8">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -694,8 +1602,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:F18">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="C13:F19">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -703,6 +1619,126 @@
         <color theme="0"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70:F74 A75:D75">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:F39 G35:G36">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79:F83 G79">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:D41 A49:D50 A56:D57 A51:A55">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44:G48">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:G39">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70:G74">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFC00000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79:G83">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>